<commit_message>
funciona scrapping con librerias descargadas nuevamente
</commit_message>
<xml_diff>
--- a/3_feature_engineering/gopro_20250210.xlsx
+++ b/3_feature_engineering/gopro_20250210.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1096049607</v>
+        <v>1100307962</v>
       </c>
       <c r="B17" t="n">
         <v>20250210</v>
@@ -1159,17 +1159,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>350,00</t>
+          <t>200,00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>good</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t xml:space="preserve">gopro hero 10 black con accesorios </t>
+          <t>gopro 10 black</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1185,13 +1185,13 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://es.wallapop.com/item/gopro-hero-10-black-con-accesorios-1096049607</t>
+          <t>https://es.wallapop.com/item/gopro-10-black-1100307962</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1086866366</v>
+        <v>1085625687</v>
       </c>
       <c r="B18" t="n">
         <v>20250210</v>
@@ -1203,17 +1203,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>250,00</t>
+          <t>375,00</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>good</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t xml:space="preserve">go pro hero 10 black </t>
+          <t>gopro hero 10 black</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1229,13 +1229,13 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://es.wallapop.com/item/go-pro-hero-10-black-1086866366</t>
+          <t>https://es.wallapop.com/item/gopro-hero-10-black-1085625687</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1080565222</v>
+        <v>1096049607</v>
       </c>
       <c r="B19" t="n">
         <v>20250210</v>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>camara go pro 10 black</t>
+          <t xml:space="preserve">gopro hero 10 black con accesorios </t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1273,51 +1273,1635 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://es.wallapop.com/item/camara-go-pro-10-black-1080565222</t>
+          <t>https://es.wallapop.com/item/gopro-hero-10-black-con-accesorios-1096049607</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
+        <v>1086866366</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>250,00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">go pro hero 10 black </t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>60</v>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/go-pro-hero-10-black-1086866366</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1080565222</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>350,00</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>camara go pro 10 black</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>60</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/camara-go-pro-10-black-1080565222</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
         <v>1030106635</v>
       </c>
-      <c r="B20" t="n">
-        <v>20250210</v>
-      </c>
-      <c r="C20" t="inlineStr">
+      <c r="B22" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C22" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>270,00</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>new</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>gopro hero 10</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>madrid</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>60</v>
-      </c>
-      <c r="I20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" t="inlineStr">
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>60</v>
+      </c>
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" t="inlineStr">
         <is>
           <t>https://es.wallapop.com/item/gopro-hero-10-1030106635</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1096323314</v>
+      </c>
+      <c r="B23" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>230,00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>gopro hero 11 black</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>60</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-11-black-1096323314</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1094638512</v>
+      </c>
+      <c r="B24" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>330,00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gopro 11 black </t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>60</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-11-black-1094638512</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1094487184</v>
+      </c>
+      <c r="B25" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>250,00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>gopro hero 11</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>60</v>
+      </c>
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-11-1094487184</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1092024308</v>
+      </c>
+      <c r="B26" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>289,00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>camara ultracompacta gopro 11 black</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>60</v>
+      </c>
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/camara-ultracompacta-gopro-11-black-1092024308</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1092221554</v>
+      </c>
+      <c r="B27" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>280,00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>gopro hero 11 sin apenas uso.</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>60</v>
+      </c>
+      <c r="I27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-11-sin-apenas-uso-1092221554</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1092505387</v>
+      </c>
+      <c r="B28" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>340,00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>gopro hero 11 black  baterias enduro</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>60</v>
+      </c>
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-11-black-y-accesorios-1092505387</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1080359690</v>
+      </c>
+      <c r="B29" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>220,00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>gopro hero 11</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>60</v>
+      </c>
+      <c r="I29" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-11-1080359690</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1074168225</v>
+      </c>
+      <c r="B30" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>400,00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>gopro hero 11 black + accesorios</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>60</v>
+      </c>
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-11-black---accesorios-1074168225</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1070264638</v>
+      </c>
+      <c r="B31" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>315,00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>gopro hero black 11 + extras</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>60</v>
+      </c>
+      <c r="I31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-11---extras-1070264638</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1065739896</v>
+      </c>
+      <c r="B32" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>300,00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>gopro 11 black + accesorios</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>60</v>
+      </c>
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-11-black---accesorios-1065739896</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1058245981</v>
+      </c>
+      <c r="B33" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>295,00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>gopro 11 hero black</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>60</v>
+      </c>
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-11-hero-black-1058245981</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1049932839</v>
+      </c>
+      <c r="B34" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>290,00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>gopro 11 black</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>60</v>
+      </c>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-11-black-1049932839</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1058979498</v>
+      </c>
+      <c r="B35" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>350,00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>cámara gopro 11 black</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>60</v>
+      </c>
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/camara-gopro-11-black-1058979498</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1044882801</v>
+      </c>
+      <c r="B36" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>350,00</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>gopro 11</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>60</v>
+      </c>
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-11-1044882801</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1041397524</v>
+      </c>
+      <c r="B37" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>240,00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>gopro 11 hero black</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>60</v>
+      </c>
+      <c r="I37" t="b">
+        <v>0</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-11-hero-black-1041397524</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1012043733</v>
+      </c>
+      <c r="B38" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>340,00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>gopro 11 +volta + media+kit como nuevo</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>60</v>
+      </c>
+      <c r="I38" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-11-kit-1012043733</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1055352107</v>
+      </c>
+      <c r="B39" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>360,00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>good</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>gopro hero 11 black</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>60</v>
+      </c>
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-11-black-1055352107</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1099417392</v>
+      </c>
+      <c r="B40" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>250,00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>gopro hero 11</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>60</v>
+      </c>
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-11-1099417392</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1094909743</v>
+      </c>
+      <c r="B41" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>270,00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>go pro hero 11 black</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>60</v>
+      </c>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/go-pro-hero-11-black-1094909743</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1094903053</v>
+      </c>
+      <c r="B42" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>270,00</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">go pro hero 11 black </t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>60</v>
+      </c>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/go-pro-hero-11-black-1094903053</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1083902061</v>
+      </c>
+      <c r="B43" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>350,00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>go pro 11 como nueva</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>60</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/go-pro-11-como-nueva-1083902061</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1061806929</v>
+      </c>
+      <c r="B44" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>360,00</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>⚠️gopro hero 11 naked nueva</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>60</v>
+      </c>
+      <c r="I44" t="b">
+        <v>0</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-11-naked-sin-usar-1061806929</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1099559245</v>
+      </c>
+      <c r="B45" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>300,00</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>gopro hero 12 black</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>60</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-12-black-1099559245</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1097081705</v>
+      </c>
+      <c r="B46" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>320,00</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gopro hero 12 black </t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>60</v>
+      </c>
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-12-black-1097081705</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1098650360</v>
+      </c>
+      <c r="B47" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>350,00</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>go pro hero 12 black</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>60</v>
+      </c>
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/go-pro-hero-12-black-1098650360</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1072590194</v>
+      </c>
+      <c r="B48" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>310,00</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>gopro 12</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>60</v>
+      </c>
+      <c r="I48" t="b">
+        <v>0</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-12-1072590194</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1050597462</v>
+      </c>
+      <c r="B49" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>300,00</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>gopro hero 12 naked</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>60</v>
+      </c>
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-12-naked-1050597462</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1066722758</v>
+      </c>
+      <c r="B50" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>325,00</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>as_good_as_new</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">go pro 12 </t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>60</v>
+      </c>
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/go-pro-12-1066722758</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1098125239</v>
+      </c>
+      <c r="B51" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>299,95</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>good</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>camara gopro hero 12 black + kit accesorios 201874</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>60</v>
+      </c>
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/camara-gopro-hero-12-black---kit-accesorios-201874-1098125239</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1094196062</v>
+      </c>
+      <c r="B52" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>280,00</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>gopro hero 12 black</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>60</v>
+      </c>
+      <c r="I52" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-12-black-1094196062</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>1081465646</v>
+      </c>
+      <c r="B53" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>390,00</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>⚠️gopro hero 12 naked nueva</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>60</v>
+      </c>
+      <c r="I53" t="b">
+        <v>0</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-12-naked-1081465646</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>1050151212</v>
+      </c>
+      <c r="B54" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>350,00</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>gopro hero 12</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>60</v>
+      </c>
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-hero-12-1050151212</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>1100412627</v>
+      </c>
+      <c r="B55" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>299,00</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>gopro 13 y sd 128gb</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>60</v>
+      </c>
+      <c r="I55" t="b">
+        <v>0</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-13-y-sd-128gb-1100412627</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>1094367879</v>
+      </c>
+      <c r="B56" t="n">
+        <v>20250210</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>350,00</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>gopro 13 black</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>madrid</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>60</v>
+      </c>
+      <c r="I56" t="b">
+        <v>0</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>https://es.wallapop.com/item/gopro-13-black-1094367879</t>
         </is>
       </c>
     </row>

</xml_diff>